<commit_message>
Addition of Wim Bonneux
</commit_message>
<xml_diff>
--- a/ICEG-PersonList.xlsx
+++ b/ICEG-PersonList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc.bruyland\OneDrive - GCloud Belgium\Documents\WG_ICEG\ICEG presentations\REV_20190913\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{D706CA44-37CC-411A-9743-1F76DFE895DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{3F871AF3-4354-4432-B786-18EBF6237471}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{D706CA44-37CC-411A-9743-1F76DFE895DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{914F178E-4371-4645-BF92-222747C1FE00}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D3D7583-45EE-49AC-A828-9EBBA903D001}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="106">
   <si>
     <t>OU</t>
   </si>
@@ -344,6 +344,15 @@
   </si>
   <si>
     <t>Community Flanders</t>
+  </si>
+  <si>
+    <t>Bonneux</t>
+  </si>
+  <si>
+    <t>Wim</t>
+  </si>
+  <si>
+    <t>wim.bonneux@minfin.fed.be</t>
   </si>
 </sst>
 </file>
@@ -482,12 +491,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74C0F28B-114B-490F-8EF4-0424BED04FA1}" name="Table1" displayName="Table1" ref="A1:E28" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E28" xr:uid="{57A42AF8-05CC-49D6-A904-FE89BF898683}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E28">
-    <sortCondition ref="A2:A28"/>
-    <sortCondition ref="B2:B28"/>
-    <sortCondition ref="C2:C28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74C0F28B-114B-490F-8EF4-0424BED04FA1}" name="Table1" displayName="Table1" ref="A1:E29" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E29" xr:uid="{57A42AF8-05CC-49D6-A904-FE89BF898683}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E29">
+    <sortCondition ref="A2:A29"/>
+    <sortCondition ref="B2:B29"/>
+    <sortCondition ref="C2:C29"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C814016B-83D5-4C38-A191-6EDBFDDCDF23}" name="OU"/>
@@ -799,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F7E18D-9D32-40EF-A662-9ECA2F934D91}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +877,7 @@
         <v>85</v>
       </c>
       <c r="G3" t="str">
-        <f>IF(D3 &lt;&gt;"tbd", G2&amp;";"&amp;D3,G2)</f>
+        <f t="shared" ref="G3:G29" si="0">IF(D3 &lt;&gt;"tbd", G2&amp;";"&amp;D3,G2)</f>
         <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be</v>
       </c>
     </row>
@@ -889,7 +898,7 @@
         <v>22</v>
       </c>
       <c r="G4" t="str">
-        <f>IF(D4 &lt;&gt;"tbd", G3&amp;";"&amp;D4,G3)</f>
+        <f t="shared" si="0"/>
         <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be</v>
       </c>
     </row>
@@ -907,7 +916,7 @@
         <v>15</v>
       </c>
       <c r="G5" t="str">
-        <f>IF(D5 &lt;&gt;"tbd", G4&amp;";"&amp;D5,G4)</f>
+        <f t="shared" si="0"/>
         <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be</v>
       </c>
     </row>
@@ -928,7 +937,7 @@
         <v>34</v>
       </c>
       <c r="G6" t="str">
-        <f>IF(D6 &lt;&gt;"tbd", G5&amp;";"&amp;D6,G5)</f>
+        <f t="shared" si="0"/>
         <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be</v>
       </c>
     </row>
@@ -937,20 +946,17 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
+        <v>104</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="G7" t="str">
-        <f>IF(D7 &lt;&gt;"tbd", G6&amp;";"&amp;D7,G6)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -958,104 +964,104 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
       <c r="G8" t="str">
-        <f>IF(D8 &lt;&gt;"tbd", G7&amp;";"&amp;D8,G7)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>82</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>79</v>
       </c>
-      <c r="G9" t="str">
-        <f>IF(D9 &lt;&gt;"tbd", G8&amp;";"&amp;D9,G8)</f>
-        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be </v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be </v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>95</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>65</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>65</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>65</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>96</v>
       </c>
-      <c r="G10" t="str">
-        <f>IF(D10 &lt;&gt;"tbd", G9&amp;";"&amp;D10,G9)</f>
-        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be </v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be </v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>75</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>74</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>73</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>76</v>
       </c>
-      <c r="G11" t="str">
-        <f>IF(D11 &lt;&gt;"tbd", G10&amp;";"&amp;D11,G10)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="G12" t="str">
-        <f>IF(D12 &lt;&gt;"tbd", G11&amp;";"&amp;D12,G11)</f>
-        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels </v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1063,59 +1069,62 @@
         <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" t="s">
-        <v>66</v>
+        <v>36</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>77</v>
       </c>
       <c r="G13" t="str">
-        <f>IF(D13 &lt;&gt;"tbd", G12&amp;";"&amp;D13,G12)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels </v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>63</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>94</v>
       </c>
-      <c r="G14" t="str">
-        <f>IF(D14 &lt;&gt;"tbd", G13&amp;";"&amp;D14,G13)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="G15" t="str">
-        <f>IF(D15 &lt;&gt;"tbd", G14&amp;";"&amp;D15,G14)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1123,35 +1132,35 @@
         <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G16" t="str">
-        <f>IF(D16 &lt;&gt;"tbd", G15&amp;";"&amp;D16,G15)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G17" t="str">
-        <f>IF(D17 &lt;&gt;"tbd", G16&amp;";"&amp;D17,G16)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1159,203 +1168,200 @@
         <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G18" t="str">
-        <f>IF(D18 &lt;&gt;"tbd", G17&amp;";"&amp;D18,G17)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="G19" t="str">
-        <f>IF(D19 &lt;&gt;"tbd", G18&amp;";"&amp;D19,G18)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="G20" t="str">
-        <f>IF(D20 &lt;&gt;"tbd", G19&amp;";"&amp;D20,G19)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
+      <c r="B21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
         <v>33</v>
       </c>
       <c r="G21" t="str">
-        <f>IF(D21 &lt;&gt;"tbd", G20&amp;";"&amp;D21,G20)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>41</v>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
       </c>
       <c r="G22" t="str">
-        <f>IF(D22 &lt;&gt;"tbd", G21&amp;";"&amp;D22,G21)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>61</v>
+        <v>32</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
       </c>
       <c r="G23" t="str">
-        <f>IF(D23 &lt;&gt;"tbd", G22&amp;";"&amp;D23,G22)</f>
-        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels </v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" t="s">
-        <v>33</v>
+        <v>58</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="G24" t="str">
-        <f>IF(D24 &lt;&gt;"tbd", G23&amp;";"&amp;D24,G23)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels </v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
       </c>
       <c r="G25" t="str">
-        <f>IF(D25 &lt;&gt;"tbd", G24&amp;";"&amp;D25,G24)</f>
-        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be </v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="E26" t="s">
         <v>33</v>
       </c>
       <c r="G26" t="str">
-        <f>IF(D26 &lt;&gt;"tbd", G25&amp;";"&amp;D26,G25)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be </v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>53</v>
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
       </c>
       <c r="G27" t="str">
-        <f>IF(D27 &lt;&gt;"tbd", G26&amp;";"&amp;D27,G26)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1363,20 +1369,41 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>53</v>
       </c>
       <c r="G28" t="str">
-        <f>IF(D28 &lt;&gt;"tbd", G27&amp;";"&amp;D28,G27)</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="315" x14ac:dyDescent="0.25">
@@ -1384,35 +1411,23 @@
         <v>92</v>
       </c>
       <c r="D32" s="5" t="str">
-        <f>G28</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
+        <f>G29</f>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" display="mailto:wim.bonneux@minfin.fed.be" xr:uid="{2433AB49-3546-47F5-B4BE-52BA6E657B1C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004737C511A6E23947AD14508ECFA660DC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0dac2bd4b9910dbc7ba732ce23202609">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5b340481-ff30-4157-987a-05f8c1c3754a" xmlns:ns4="c1fa55ad-f680-4b5e-b0c5-c910667318ab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85b5d4cdc5a71fa11467f17736926f78" ns3:_="" ns4:_="">
     <xsd:import namespace="5b340481-ff30-4157-987a-05f8c1c3754a"/>
@@ -1615,32 +1630,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1453B941-BB20-4C76-8540-80BBC435E41D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c1fa55ad-f680-4b5e-b0c5-c910667318ab"/>
-    <ds:schemaRef ds:uri="5b340481-ff30-4157-987a-05f8c1c3754a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{407D0A84-4765-4B8B-8260-B6BFA4338C6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9A45D31-968B-45E6-B89B-4586A18391BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1657,4 +1662,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{407D0A84-4765-4B8B-8260-B6BFA4338C6E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1453B941-BB20-4C76-8540-80BBC435E41D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="c1fa55ad-f680-4b5e-b0c5-c910667318ab"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5b340481-ff30-4157-987a-05f8c1c3754a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>